<commit_message>
Deploying to gh-pages from @ Healthedata1/test-stuff@cd5b847990ada2b89f3809ba490374934f62ea14 🚀
</commit_message>
<xml_diff>
--- a/all-profiles.xlsx
+++ b/all-profiles.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5101" uniqueCount="667">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5602" uniqueCount="711">
   <si>
     <t>Property</t>
   </si>
@@ -2113,6 +2113,142 @@
     <t>This might not include provenances for all versions of the request – only those deemed “relevant” or important. This SHALL NOT include the Provenance associated with this current version of the resource.  (If that provenance is deemed to be a “relevant” change, it will need to be added as part of a later update.  Until then, it can be queried directly as the Provenance that points to this version using _revinclude All Provenances should have some historical version of this Request as their subject.</t>
+  </si>
+  <si>
+    <t>test-binding</t>
+  </si>
+  <si>
+    <t>http://example.org/fhir/StructureDefinition/test-binding</t>
+  </si>
+  <si>
+    <t>TestBinding</t>
+  </si>
+  <si>
+    <t>Test Binding</t>
+  </si>
+  <si>
+    <t>2025-08-22</t>
+  </si>
+  <si>
+    <t>A profile on the FHIR R4 Basic resource for representing a referral, with the code element constrained to the LOINC valid HL7 attachment requests value set.</t>
+  </si>
+  <si>
+    <t>Basic</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/StructureDefinition/Basic</t>
+  </si>
+  <si>
+    <t>Z-resource
+Extension-resourceCustom-resource</t>
+  </si>
+  <si>
+    <t>Referral Basic Profile</t>
+  </si>
+  <si>
+    <t>A profile on Basic resource for representing referral information.</t>
+  </si>
+  <si>
+    <t>Basic.id</t>
+  </si>
+  <si>
+    <t>Basic.meta</t>
+  </si>
+  <si>
+    <t>Basic.implicitRules</t>
+  </si>
+  <si>
+    <t>Basic.language</t>
+  </si>
+  <si>
+    <t>Basic.text</t>
+  </si>
+  <si>
+    <t>Basic.contained</t>
+  </si>
+  <si>
+    <t>Basic.extension</t>
+  </si>
+  <si>
+    <t>Basic.modifierExtension</t>
+  </si>
+  <si>
+    <t>Basic.identifier</t>
+  </si>
+  <si>
+    <t>Business identifier</t>
+  </si>
+  <si>
+    <t>Identifier assigned to the resource for business purposes, outside the context of FHIR.</t>
+  </si>
+  <si>
+    <t>Basic.code</t>
+  </si>
+  <si>
+    <t>Kind of attachment</t>
+  </si>
+  <si>
+    <t>constrained to valid HL7 attachment request codes from LOINC.</t>
+  </si>
+  <si>
+    <t>Because resource references will only be able to indicate 'Basic', the type of reference will need to be specified in a Profile identified as part of the resource.  Refer to the resource notes section for information on appropriate terminologies for this code.
+This element is labeled as a modifier because it defines the meaning of the resource and cannot be ignored.</t>
+  </si>
+  <si>
+    <t>Must be able to distinguish different types of Basic resources.</t>
+  </si>
+  <si>
+    <t>bound to LOINC valid HL7 attachment requests.</t>
+  </si>
+  <si>
+    <t>http://loinc.org/vs/valid-hl7-attachment-requests</t>
+  </si>
+  <si>
+    <t>Basic.subject</t>
+  </si>
+  <si>
+    <t>Identifies the focus of this resource</t>
+  </si>
+  <si>
+    <t>Identifies the patient, practitioner, device or any other resource that is the "focus" of this resource.</t>
+  </si>
+  <si>
+    <t>Optional as not all potential resources will have subjects.  Resources associated with multiple subjects can handle this via extension.</t>
+  </si>
+  <si>
+    <t>Needed for partitioning the resource by Patient.</t>
+  </si>
+  <si>
+    <t>Basic.created</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date
+</t>
+  </si>
+  <si>
+    <t>When created</t>
+  </si>
+  <si>
+    <t>Identifies when the resource was first created.</t>
+  </si>
+  <si>
+    <t>Allows ordering resource instances by time.</t>
+  </si>
+  <si>
+    <t>Basic.author</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference(Practitioner|4.0.1|PractitionerRole|4.0.1|Patient|4.0.1|RelatedPerson|4.0.1|Organization|4.0.1)
+</t>
+  </si>
+  <si>
+    <t>Who created</t>
+  </si>
+  <si>
+    <t>Indicates who was responsible for creating the resource instance.</t>
+  </si>
+  <si>
+    <t>Needed for partitioning the resource.</t>
   </si>
 </sst>
 </file>
@@ -2246,7 +2382,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B94"/>
+  <dimension ref="A1:B115"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -2990,6 +3126,168 @@
         <v>38</v>
       </c>
     </row>
+    <row r="95">
+      <c r="A95" t="s" s="1">
+        <v>0</v>
+      </c>
+      <c r="B95" t="s" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="s" s="2">
+        <v>2</v>
+      </c>
+      <c r="B96" t="s" s="2">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="s" s="2">
+        <v>4</v>
+      </c>
+      <c r="B97" t="s" s="2">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="s" s="2">
+        <v>6</v>
+      </c>
+      <c r="B98" t="s" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="B99" t="s" s="2">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="B100" t="s" s="2">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="s" s="2">
+        <v>12</v>
+      </c>
+      <c r="B101" t="s" s="2">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="B102" s="2"/>
+    </row>
+    <row r="103">
+      <c r="A103" t="s" s="2">
+        <v>16</v>
+      </c>
+      <c r="B103" t="s" s="2">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="B104" t="s" s="2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="B105" t="s" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="s" s="2">
+        <v>22</v>
+      </c>
+      <c r="B106" t="s" s="2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="s" s="2">
+        <v>24</v>
+      </c>
+      <c r="B107" t="s" s="2">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="s" s="2">
+        <v>26</v>
+      </c>
+      <c r="B108" s="2"/>
+    </row>
+    <row r="109">
+      <c r="A109" t="s" s="2">
+        <v>27</v>
+      </c>
+      <c r="B109" s="2"/>
+    </row>
+    <row r="110">
+      <c r="A110" t="s" s="2">
+        <v>28</v>
+      </c>
+      <c r="B110" t="s" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="s" s="2">
+        <v>30</v>
+      </c>
+      <c r="B111" t="s" s="2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="s" s="2">
+        <v>32</v>
+      </c>
+      <c r="B112" t="s" s="2">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="B113" t="s" s="2">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="B114" t="s" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="B115" t="s" s="2">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -2997,7 +3295,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AK149"/>
+  <dimension ref="A1:AK163"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -18628,6 +18926,1476 @@
         <v>96</v>
       </c>
     </row>
+    <row r="150">
+      <c r="A150" t="s" s="2">
+        <v>667</v>
+      </c>
+      <c r="B150" t="s" s="2">
+        <v>673</v>
+      </c>
+      <c r="C150" t="s" s="2">
+        <v>673</v>
+      </c>
+      <c r="D150" s="2"/>
+      <c r="E150" t="s" s="2">
+        <v>675</v>
+      </c>
+      <c r="F150" s="2"/>
+      <c r="G150" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="H150" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="I150" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="J150" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="K150" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="L150" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="M150" t="s" s="2">
+        <v>676</v>
+      </c>
+      <c r="N150" t="s" s="2">
+        <v>677</v>
+      </c>
+      <c r="O150" s="2"/>
+      <c r="P150" s="2"/>
+      <c r="Q150" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="R150" s="2"/>
+      <c r="S150" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="T150" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="U150" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="V150" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="W150" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="X150" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Y150" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Z150" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AA150" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AB150" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AC150" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AD150" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AE150" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AF150" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AG150" t="s" s="2">
+        <v>673</v>
+      </c>
+      <c r="AH150" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AI150" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AJ150" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AK150" t="s" s="2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="s" s="2">
+        <v>667</v>
+      </c>
+      <c r="B151" t="s" s="2">
+        <v>678</v>
+      </c>
+      <c r="C151" t="s" s="2">
+        <v>678</v>
+      </c>
+      <c r="D151" s="2"/>
+      <c r="E151" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="F151" s="2"/>
+      <c r="G151" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="H151" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="I151" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="J151" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="K151" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="L151" t="s" s="2">
+        <v>86</v>
+      </c>
+      <c r="M151" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="N151" t="s" s="2">
+        <v>88</v>
+      </c>
+      <c r="O151" t="s" s="2">
+        <v>89</v>
+      </c>
+      <c r="P151" s="2"/>
+      <c r="Q151" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="R151" s="2"/>
+      <c r="S151" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="T151" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="U151" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="V151" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="W151" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="X151" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Y151" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Z151" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AA151" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AB151" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AC151" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AD151" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AE151" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AF151" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AG151" t="s" s="2">
+        <v>90</v>
+      </c>
+      <c r="AH151" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AI151" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AJ151" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AK151" t="s" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="s" s="2">
+        <v>667</v>
+      </c>
+      <c r="B152" t="s" s="2">
+        <v>679</v>
+      </c>
+      <c r="C152" t="s" s="2">
+        <v>679</v>
+      </c>
+      <c r="D152" s="2"/>
+      <c r="E152" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="F152" s="2"/>
+      <c r="G152" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="H152" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="I152" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="J152" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="K152" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="L152" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="M152" t="s" s="2">
+        <v>93</v>
+      </c>
+      <c r="N152" t="s" s="2">
+        <v>94</v>
+      </c>
+      <c r="O152" s="2"/>
+      <c r="P152" s="2"/>
+      <c r="Q152" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="R152" s="2"/>
+      <c r="S152" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="T152" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="U152" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="V152" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="W152" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="X152" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Y152" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Z152" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AA152" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AB152" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AC152" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AD152" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AE152" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AF152" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AG152" t="s" s="2">
+        <v>95</v>
+      </c>
+      <c r="AH152" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AI152" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AJ152" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AK152" t="s" s="2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="s" s="2">
+        <v>667</v>
+      </c>
+      <c r="B153" t="s" s="2">
+        <v>680</v>
+      </c>
+      <c r="C153" t="s" s="2">
+        <v>680</v>
+      </c>
+      <c r="D153" s="2"/>
+      <c r="E153" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="F153" s="2"/>
+      <c r="G153" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="H153" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="I153" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="J153" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="K153" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="L153" t="s" s="2">
+        <v>98</v>
+      </c>
+      <c r="M153" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="N153" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="O153" t="s" s="2">
+        <v>101</v>
+      </c>
+      <c r="P153" s="2"/>
+      <c r="Q153" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="R153" s="2"/>
+      <c r="S153" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="T153" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="U153" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="V153" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="W153" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="X153" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Y153" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Z153" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AA153" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AB153" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AC153" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AD153" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AE153" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AF153" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AG153" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="AH153" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AI153" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AJ153" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AK153" t="s" s="2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="s" s="2">
+        <v>667</v>
+      </c>
+      <c r="B154" t="s" s="2">
+        <v>681</v>
+      </c>
+      <c r="C154" t="s" s="2">
+        <v>681</v>
+      </c>
+      <c r="D154" s="2"/>
+      <c r="E154" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="F154" s="2"/>
+      <c r="G154" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="H154" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="I154" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="J154" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="K154" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="L154" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="M154" t="s" s="2">
+        <v>105</v>
+      </c>
+      <c r="N154" t="s" s="2">
+        <v>106</v>
+      </c>
+      <c r="O154" t="s" s="2">
+        <v>107</v>
+      </c>
+      <c r="P154" s="2"/>
+      <c r="Q154" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="R154" s="2"/>
+      <c r="S154" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="T154" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="U154" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="V154" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="W154" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="X154" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Y154" t="s" s="2">
+        <v>108</v>
+      </c>
+      <c r="Z154" t="s" s="2">
+        <v>109</v>
+      </c>
+      <c r="AA154" t="s" s="2">
+        <v>110</v>
+      </c>
+      <c r="AB154" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AC154" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AD154" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AE154" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AF154" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AG154" t="s" s="2">
+        <v>111</v>
+      </c>
+      <c r="AH154" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AI154" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AJ154" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AK154" t="s" s="2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="s" s="2">
+        <v>667</v>
+      </c>
+      <c r="B155" t="s" s="2">
+        <v>682</v>
+      </c>
+      <c r="C155" t="s" s="2">
+        <v>682</v>
+      </c>
+      <c r="D155" s="2"/>
+      <c r="E155" t="s" s="2">
+        <v>113</v>
+      </c>
+      <c r="F155" s="2"/>
+      <c r="G155" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="H155" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="I155" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="J155" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="K155" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="L155" t="s" s="2">
+        <v>114</v>
+      </c>
+      <c r="M155" t="s" s="2">
+        <v>115</v>
+      </c>
+      <c r="N155" t="s" s="2">
+        <v>116</v>
+      </c>
+      <c r="O155" t="s" s="2">
+        <v>117</v>
+      </c>
+      <c r="P155" s="2"/>
+      <c r="Q155" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="R155" s="2"/>
+      <c r="S155" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="T155" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="U155" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="V155" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="W155" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="X155" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Y155" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Z155" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AA155" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AB155" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AC155" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AD155" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AE155" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AF155" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AG155" t="s" s="2">
+        <v>118</v>
+      </c>
+      <c r="AH155" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AI155" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AJ155" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AK155" t="s" s="2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="s" s="2">
+        <v>667</v>
+      </c>
+      <c r="B156" t="s" s="2">
+        <v>683</v>
+      </c>
+      <c r="C156" t="s" s="2">
+        <v>683</v>
+      </c>
+      <c r="D156" s="2"/>
+      <c r="E156" t="s" s="2">
+        <v>120</v>
+      </c>
+      <c r="F156" s="2"/>
+      <c r="G156" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="H156" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="I156" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="J156" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="K156" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="L156" t="s" s="2">
+        <v>121</v>
+      </c>
+      <c r="M156" t="s" s="2">
+        <v>122</v>
+      </c>
+      <c r="N156" t="s" s="2">
+        <v>123</v>
+      </c>
+      <c r="O156" t="s" s="2">
+        <v>124</v>
+      </c>
+      <c r="P156" s="2"/>
+      <c r="Q156" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="R156" s="2"/>
+      <c r="S156" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="T156" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="U156" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="V156" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="W156" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="X156" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Y156" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Z156" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AA156" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AB156" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AC156" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AD156" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AE156" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AF156" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AG156" t="s" s="2">
+        <v>125</v>
+      </c>
+      <c r="AH156" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AI156" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AJ156" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AK156" t="s" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="s" s="2">
+        <v>667</v>
+      </c>
+      <c r="B157" t="s" s="2">
+        <v>684</v>
+      </c>
+      <c r="C157" t="s" s="2">
+        <v>684</v>
+      </c>
+      <c r="D157" s="2"/>
+      <c r="E157" t="s" s="2">
+        <v>141</v>
+      </c>
+      <c r="F157" s="2"/>
+      <c r="G157" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="H157" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="I157" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="J157" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="K157" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="L157" t="s" s="2">
+        <v>127</v>
+      </c>
+      <c r="M157" t="s" s="2">
+        <v>226</v>
+      </c>
+      <c r="N157" t="s" s="2">
+        <v>466</v>
+      </c>
+      <c r="O157" t="s" s="2">
+        <v>144</v>
+      </c>
+      <c r="P157" s="2"/>
+      <c r="Q157" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="R157" s="2"/>
+      <c r="S157" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="T157" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="U157" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="V157" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="W157" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="X157" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Y157" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Z157" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AA157" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AB157" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AC157" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AD157" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AE157" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AF157" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AG157" t="s" s="2">
+        <v>132</v>
+      </c>
+      <c r="AH157" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AI157" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AJ157" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AK157" t="s" s="2">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="s" s="2">
+        <v>667</v>
+      </c>
+      <c r="B158" t="s" s="2">
+        <v>685</v>
+      </c>
+      <c r="C158" t="s" s="2">
+        <v>685</v>
+      </c>
+      <c r="D158" s="2"/>
+      <c r="E158" t="s" s="2">
+        <v>141</v>
+      </c>
+      <c r="F158" s="2"/>
+      <c r="G158" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="H158" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="I158" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="J158" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="K158" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="L158" t="s" s="2">
+        <v>127</v>
+      </c>
+      <c r="M158" t="s" s="2">
+        <v>142</v>
+      </c>
+      <c r="N158" t="s" s="2">
+        <v>143</v>
+      </c>
+      <c r="O158" t="s" s="2">
+        <v>144</v>
+      </c>
+      <c r="P158" t="s" s="2">
+        <v>145</v>
+      </c>
+      <c r="Q158" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="R158" s="2"/>
+      <c r="S158" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="T158" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="U158" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="V158" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="W158" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="X158" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Y158" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Z158" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AA158" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AB158" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AC158" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AD158" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AE158" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AF158" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AG158" t="s" s="2">
+        <v>146</v>
+      </c>
+      <c r="AH158" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AI158" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AJ158" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AK158" t="s" s="2">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="s" s="2">
+        <v>667</v>
+      </c>
+      <c r="B159" t="s" s="2">
+        <v>686</v>
+      </c>
+      <c r="C159" t="s" s="2">
+        <v>686</v>
+      </c>
+      <c r="D159" s="2"/>
+      <c r="E159" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="F159" s="2"/>
+      <c r="G159" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="H159" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="I159" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="J159" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="K159" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="L159" t="s" s="2">
+        <v>148</v>
+      </c>
+      <c r="M159" t="s" s="2">
+        <v>687</v>
+      </c>
+      <c r="N159" t="s" s="2">
+        <v>688</v>
+      </c>
+      <c r="O159" s="2"/>
+      <c r="P159" s="2"/>
+      <c r="Q159" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="R159" s="2"/>
+      <c r="S159" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="T159" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="U159" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="V159" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="W159" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="X159" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Y159" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Z159" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AA159" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AB159" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AC159" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AD159" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AE159" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AF159" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AG159" t="s" s="2">
+        <v>686</v>
+      </c>
+      <c r="AH159" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AI159" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="AJ159" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AK159" t="s" s="2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="s" s="2">
+        <v>667</v>
+      </c>
+      <c r="B160" t="s" s="2">
+        <v>689</v>
+      </c>
+      <c r="C160" t="s" s="2">
+        <v>689</v>
+      </c>
+      <c r="D160" s="2"/>
+      <c r="E160" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="F160" s="2"/>
+      <c r="G160" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="H160" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="I160" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="J160" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="K160" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="L160" t="s" s="2">
+        <v>169</v>
+      </c>
+      <c r="M160" t="s" s="2">
+        <v>690</v>
+      </c>
+      <c r="N160" t="s" s="2">
+        <v>691</v>
+      </c>
+      <c r="O160" t="s" s="2">
+        <v>692</v>
+      </c>
+      <c r="P160" t="s" s="2">
+        <v>693</v>
+      </c>
+      <c r="Q160" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="R160" s="2"/>
+      <c r="S160" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="T160" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="U160" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="V160" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="W160" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="X160" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Y160" t="s" s="2">
+        <v>160</v>
+      </c>
+      <c r="Z160" t="s" s="2">
+        <v>694</v>
+      </c>
+      <c r="AA160" t="s" s="2">
+        <v>695</v>
+      </c>
+      <c r="AB160" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AC160" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AD160" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AE160" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AF160" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AG160" t="s" s="2">
+        <v>689</v>
+      </c>
+      <c r="AH160" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AI160" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AJ160" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AK160" t="s" s="2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="s" s="2">
+        <v>667</v>
+      </c>
+      <c r="B161" t="s" s="2">
+        <v>696</v>
+      </c>
+      <c r="C161" t="s" s="2">
+        <v>696</v>
+      </c>
+      <c r="D161" s="2"/>
+      <c r="E161" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="F161" s="2"/>
+      <c r="G161" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="H161" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="I161" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="J161" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="K161" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="L161" t="s" s="2">
+        <v>370</v>
+      </c>
+      <c r="M161" t="s" s="2">
+        <v>697</v>
+      </c>
+      <c r="N161" t="s" s="2">
+        <v>698</v>
+      </c>
+      <c r="O161" t="s" s="2">
+        <v>699</v>
+      </c>
+      <c r="P161" t="s" s="2">
+        <v>700</v>
+      </c>
+      <c r="Q161" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="R161" s="2"/>
+      <c r="S161" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="T161" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="U161" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="V161" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="W161" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="X161" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Y161" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Z161" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AA161" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AB161" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AC161" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AD161" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AE161" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AF161" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AG161" t="s" s="2">
+        <v>696</v>
+      </c>
+      <c r="AH161" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AI161" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AJ161" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AK161" t="s" s="2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="s" s="2">
+        <v>667</v>
+      </c>
+      <c r="B162" t="s" s="2">
+        <v>701</v>
+      </c>
+      <c r="C162" t="s" s="2">
+        <v>701</v>
+      </c>
+      <c r="D162" s="2"/>
+      <c r="E162" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="F162" s="2"/>
+      <c r="G162" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="H162" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="I162" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="J162" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="K162" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="L162" t="s" s="2">
+        <v>702</v>
+      </c>
+      <c r="M162" t="s" s="2">
+        <v>703</v>
+      </c>
+      <c r="N162" t="s" s="2">
+        <v>704</v>
+      </c>
+      <c r="O162" s="2"/>
+      <c r="P162" t="s" s="2">
+        <v>705</v>
+      </c>
+      <c r="Q162" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="R162" s="2"/>
+      <c r="S162" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="T162" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="U162" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="V162" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="W162" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="X162" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Y162" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Z162" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AA162" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AB162" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AC162" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AD162" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AE162" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AF162" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AG162" t="s" s="2">
+        <v>701</v>
+      </c>
+      <c r="AH162" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AI162" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AJ162" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AK162" t="s" s="2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="s" s="2">
+        <v>667</v>
+      </c>
+      <c r="B163" t="s" s="2">
+        <v>706</v>
+      </c>
+      <c r="C163" t="s" s="2">
+        <v>706</v>
+      </c>
+      <c r="D163" s="2"/>
+      <c r="E163" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="F163" s="2"/>
+      <c r="G163" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="H163" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="I163" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="J163" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="K163" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="L163" t="s" s="2">
+        <v>707</v>
+      </c>
+      <c r="M163" t="s" s="2">
+        <v>708</v>
+      </c>
+      <c r="N163" t="s" s="2">
+        <v>709</v>
+      </c>
+      <c r="O163" s="2"/>
+      <c r="P163" t="s" s="2">
+        <v>710</v>
+      </c>
+      <c r="Q163" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="R163" s="2"/>
+      <c r="S163" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="T163" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="U163" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="V163" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="W163" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="X163" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Y163" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="Z163" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AA163" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AB163" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AC163" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AD163" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AE163" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AF163" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AG163" t="s" s="2">
+        <v>706</v>
+      </c>
+      <c r="AH163" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="AI163" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="AJ163" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="AK163" t="s" s="2">
+        <v>96</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>